<commit_message>
Fix checks, json schema and examples
</commit_message>
<xml_diff>
--- a/examples/palabra/labs/lab2/lab2_result.xlsx
+++ b/examples/palabra/labs/lab2/lab2_result.xlsx
@@ -444,17 +444,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>392</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>333</t>
+          <t>357</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>35</t>
         </is>
       </c>
     </row>
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C351"/>
+  <dimension ref="A1:C393"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -667,7 +667,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Checking collision domain `A`</t>
+          <t>Checking the collision domain attached to interface `eth0` of `root`</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -684,7 +684,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Checking collision domain `C`</t>
+          <t>Checking the collision domain attached to interface `eth0` of `as1r2`</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -701,7 +701,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Checking collision domain `B`</t>
+          <t>Checking the collision domain attached to interface `eth1` of `as1r2`</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -718,7 +718,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Checking collision domain `D`</t>
+          <t>Checking the collision domain attached to interface `eth2` of `as1r2`</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -735,7 +735,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Checking collision domain `G`</t>
+          <t>Checking the collision domain attached to interface `eth0` of `as1r1`</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -752,7 +752,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Checking collision domain `F`</t>
+          <t>Checking the collision domain attached to interface `eth1` of `as1r1`</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -769,7 +769,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Checking collision domain `H`</t>
+          <t>Checking the collision domain attached to interface `eth0` of `as2r1`</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -786,7 +786,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Checking collision domain `E`</t>
+          <t>Checking the collision domain attached to interface `eth1` of `as2r1`</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -803,7 +803,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Checking collision domain `I`</t>
+          <t>Checking the collision domain attached to interface `eth2` of `as2r1`</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Checking collision domain `K`</t>
+          <t>Checking the collision domain attached to interface `eth0` of `as2r2`</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -837,7 +837,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Checking collision domain `J`</t>
+          <t>Checking the collision domain attached to interface `eth1` of `as2r2`</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Check existence of `as1r1.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth2` of `as2r2`</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -871,7 +871,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Check existence of `as1r2.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth3` of `as2r2`</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -888,7 +888,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Check existence of `as2r1.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth0` of `net`</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -905,7 +905,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Check existence of `as2r2.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth0` of `as3r1`</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -922,7 +922,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Check existence of `as3r1.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth1` of `as3r1`</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -939,7 +939,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Check existence of `as3r2.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth0` of `as3r2`</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -956,7 +956,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Check existence of `root.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth1` of `as3r2`</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Check existence of `local.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth2` of `as3r2`</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -990,7 +990,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Check existence of `pc.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth3` of `as3r2`</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1007,7 +1007,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Check existence of `net.startup` file</t>
+          <t>Checking the collision domain attached to interface `eth0` of `pc`</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Verifying the IP address (10.20.0.1/30) assigned to eth0 of as1r1</t>
+          <t>Checking the collision domain attached to interface `eth0` of `local`</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1041,7 +1041,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Verifying the IP address (1.0.0.1/24) assigned to eth1 of as1r1</t>
+          <t>Check existence of `as1r1.startup` file</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Verifying the IP address (1.1.0.1/24) assigned to eth0 of as1r2</t>
+          <t>Check existence of `as1r2.startup` file</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1075,7 +1075,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Verifying the IP address (1.0.0.2/24) assigned to eth1 of as1r2</t>
+          <t>Check existence of `as2r1.startup` file</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1092,7 +1092,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Verifying the IP address (10.20.1.1/30) assigned to eth2 of as1r2</t>
+          <t>Check existence of `as2r2.startup` file</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1109,7 +1109,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Verifying the IP address (10.20.0.2/30) assigned to eth0 of as2r1</t>
+          <t>Check existence of `as3r1.startup` file</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1126,7 +1126,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Verifying the IP address (20.30.0.1/30) assigned to eth1 of as2r1</t>
+          <t>Check existence of `as3r2.startup` file</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1143,7 +1143,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Verifying the IP address (2.0.0.1/24) assigned to eth2 of as2r1</t>
+          <t>Check existence of `root.startup` file</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1160,7 +1160,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Verifying the IP address (10.20.1.2/30) assigned to eth0 of as2r2</t>
+          <t>Check existence of `local.startup` file</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1177,7 +1177,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Verifying the IP address (2.0.0.2/24) assigned to eth1 of as2r2</t>
+          <t>Check existence of `pc.startup` file</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1194,7 +1194,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Verifying the IP address (20.30.1.1/30) assigned to eth2 of as2r2</t>
+          <t>Check existence of `net.startup` file</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1211,7 +1211,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Verifying the IP address (2.1.0.1/24) assigned to eth3 of as2r2</t>
+          <t>Verifying the IP address (10.20.0.1/30) assigned to eth0 of as1r1</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Verifying the IP address (20.30.0.2/30) assigned to eth0 of as3r1</t>
+          <t>Verifying the IP address (1.0.0.1/24) assigned to eth1 of as1r1</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1245,7 +1245,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Verifying the IP address (3.0.0.1/24) assigned to eth1 of as3r1</t>
+          <t>Verifying the IP address (1.1.0.1/24) assigned to eth0 of as1r2</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1262,7 +1262,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Verifying the IP address (20.30.1.2/30) assigned to eth0 of as3r2</t>
+          <t>Verifying the IP address (1.0.0.2/24) assigned to eth1 of as1r2</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1279,7 +1279,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Verifying the IP address (3.0.0.2/24) assigned to eth1 of as3r2</t>
+          <t>Verifying the IP address (10.20.1.1/30) assigned to eth2 of as1r2</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1296,7 +1296,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Verifying the IP address (3.2.0.1/24) assigned to eth2 of as3r2</t>
+          <t>Verifying the IP address (10.20.0.2/30) assigned to eth0 of as2r1</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1313,7 +1313,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Verifying the IP address (3.1.0.1/24) assigned to eth3 of as3r2</t>
+          <t>Verifying the IP address (20.30.0.1/30) assigned to eth1 of as2r1</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1330,7 +1330,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Verifying the IP address (1.1.0.2/24) assigned to eth0 of root</t>
+          <t>Verifying the IP address (2.0.0.1/24) assigned to eth2 of as2r1</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1347,7 +1347,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Verifying the IP address (2.1.0.2/24) assigned to eth0 of net</t>
+          <t>Verifying the IP address (10.20.1.2/30) assigned to eth0 of as2r2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1364,7 +1364,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Verifying the IP address (3.2.0.2/24) assigned to eth0 of local</t>
+          <t>Verifying the IP address (2.0.0.2/24) assigned to eth1 of as2r2</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1381,7 +1381,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Verifying the IP address (3.1.0.2/24) assigned to eth0 of pc</t>
+          <t>Verifying the IP address (20.30.1.1/30) assigned to eth2 of as2r2</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1398,7 +1398,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (2.1.0.1/24) assigned to eth3 of as2r2</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1415,7 +1415,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (20.30.0.2/30) assigned to eth0 of as3r1</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1432,7 +1432,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (3.0.0.1/24) assigned to eth1 of as3r1</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1449,7 +1449,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (20.30.1.2/30) assigned to eth0 of as3r2</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1466,7 +1466,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (3.0.0.2/24) assigned to eth1 of as3r2</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1483,7 +1483,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (3.2.0.1/24) assigned to eth2 of as3r2</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1500,7 +1500,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (3.1.0.1/24) assigned to eth3 of as3r2</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1517,7 +1517,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (1.1.0.2/24) assigned to eth0 of root</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1534,7 +1534,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (2.1.0.2/24) assigned to eth0 of net</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1551,7 +1551,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (3.2.0.2/24) assigned to eth0 of local</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `as1r1`</t>
+          <t>Verifying the IP address (3.1.0.2/24) assigned to eth0 of pc</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1585,7 +1585,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as1r1`</t>
+          <t>Verifying `1.0.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1602,7 +1602,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as1r1`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1619,7 +1619,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as1r1`</t>
+          <t>Verifying `1.1.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `as1r1`</t>
+          <t>Verifying `1.1.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1653,7 +1653,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `as1r1`</t>
+          <t>Verifying `2.0.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1670,7 +1670,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `as1r1`</t>
+          <t>Verifying `2.0.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1687,7 +1687,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `as1r1`</t>
+          <t>Verifying `2.1.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1704,7 +1704,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `as1r1`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1721,7 +1721,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `as1r1`</t>
+          <t>Verifying `3.0.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1738,7 +1738,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `as1r1`</t>
+          <t>Verifying `3.0.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1755,7 +1755,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `as1r1`</t>
+          <t>Verifying `3.1.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1772,7 +1772,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1789,7 +1789,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1806,7 +1806,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1823,7 +1823,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `10.20.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `10.20.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1857,7 +1857,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `10.20.1.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1874,7 +1874,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `10.20.1.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1891,7 +1891,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `20.30.0.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `20.30.0.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1925,7 +1925,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `20.30.1.1` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1942,7 +1942,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `20.30.1.2` reachable from device `as1r1`</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1959,7 +1959,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `1.0.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1976,7 +1976,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1993,7 +1993,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `1.1.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2010,7 +2010,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `1.1.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2027,7 +2027,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `2.0.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2044,7 +2044,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `as1r2`</t>
+          <t>Verifying `2.0.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2061,7 +2061,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `as1r2`</t>
+          <t>Verifying `2.1.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2095,7 +2095,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `3.0.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2112,7 +2112,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `as1r2`</t>
+          <t>Verifying `3.0.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2129,7 +2129,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `as1r2`</t>
+          <t>Verifying `3.1.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2146,7 +2146,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2163,7 +2163,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2180,7 +2180,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2197,7 +2197,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `10.20.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `10.20.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2231,7 +2231,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `10.20.1.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2248,7 +2248,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `10.20.1.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2265,7 +2265,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `20.30.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2282,7 +2282,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `20.30.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2299,7 +2299,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `20.30.1.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2316,7 +2316,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `20.30.1.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2333,7 +2333,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `1.0.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2350,7 +2350,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2367,7 +2367,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `1.1.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2384,7 +2384,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `1.1.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -2401,7 +2401,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `2.0.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -2418,7 +2418,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `as2r1`</t>
+          <t>Verifying `2.0.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2435,7 +2435,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `as2r1`</t>
+          <t>Verifying `2.1.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2452,7 +2452,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2469,7 +2469,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `3.0.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2486,7 +2486,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `as2r1`</t>
+          <t>Verifying `3.0.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2503,7 +2503,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `as2r1`</t>
+          <t>Verifying `3.1.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2520,7 +2520,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2537,7 +2537,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2554,7 +2554,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2571,7 +2571,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `10.20.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `10.20.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2605,7 +2605,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `10.20.1.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -2622,7 +2622,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `10.20.1.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -2639,7 +2639,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `20.30.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -2656,7 +2656,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `20.30.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -2673,7 +2673,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `20.30.1.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2690,7 +2690,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `20.30.1.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -2707,7 +2707,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `1.0.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2724,7 +2724,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -2741,7 +2741,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `1.1.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -2758,7 +2758,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `1.1.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2775,7 +2775,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `2.0.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2792,7 +2792,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `as2r2`</t>
+          <t>Verifying `2.0.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2809,7 +2809,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `as2r2`</t>
+          <t>Verifying `2.1.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2826,7 +2826,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2843,7 +2843,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `3.0.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2860,7 +2860,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `as2r2`</t>
+          <t>Verifying `3.0.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2877,7 +2877,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `as2r2`</t>
+          <t>Verifying `3.1.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2894,7 +2894,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2911,7 +2911,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2928,7 +2928,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -2945,7 +2945,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `10.20.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -2962,7 +2962,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `10.20.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2979,7 +2979,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `10.20.1.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2996,7 +2996,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `10.20.1.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -3013,7 +3013,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `20.30.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -3030,7 +3030,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `20.30.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3047,7 +3047,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `20.30.1.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -3064,7 +3064,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `20.30.1.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -3081,7 +3081,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `1.0.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -3115,7 +3115,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `1.1.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -3132,7 +3132,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `1.1.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -3149,7 +3149,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `2.0.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -3166,7 +3166,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `as3r1`</t>
+          <t>Verifying `2.0.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -3183,7 +3183,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `as3r1`</t>
+          <t>Verifying `2.1.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -3200,7 +3200,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -3217,7 +3217,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `3.0.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3234,7 +3234,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `as3r1`</t>
+          <t>Verifying `3.0.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -3251,7 +3251,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `as3r1`</t>
+          <t>Verifying `3.1.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -3268,7 +3268,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -3285,7 +3285,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -3302,7 +3302,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -3319,7 +3319,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `10.20.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -3336,7 +3336,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `10.20.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -3353,7 +3353,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `10.20.1.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `10.20.1.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -3387,7 +3387,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `20.30.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -3404,7 +3404,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `20.30.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -3421,7 +3421,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `20.30.1.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `20.30.1.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `1.0.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -3472,7 +3472,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -3489,7 +3489,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `1.1.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -3506,7 +3506,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `1.1.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -3523,7 +3523,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `2.0.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -3540,7 +3540,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `as3r2`</t>
+          <t>Verifying `2.0.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -3557,7 +3557,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `as3r2`</t>
+          <t>Verifying `2.1.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -3574,7 +3574,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -3591,7 +3591,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `3.0.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `as3r2`</t>
+          <t>Verifying `3.0.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -3625,7 +3625,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `as3r2`</t>
+          <t>Verifying `3.1.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -3642,7 +3642,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `local`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -3659,7 +3659,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `local`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -3676,7 +3676,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `local`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -3693,7 +3693,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `local`</t>
+          <t>Verifying `10.20.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -3710,7 +3710,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `local`</t>
+          <t>Verifying `10.20.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -3727,7 +3727,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `local`</t>
+          <t>Verifying `10.20.1.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -3744,7 +3744,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `local`</t>
+          <t>Verifying `10.20.1.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -3761,7 +3761,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `local`</t>
+          <t>Verifying `20.30.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -3778,7 +3778,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `local`</t>
+          <t>Verifying `20.30.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -3795,7 +3795,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `local`</t>
+          <t>Verifying `20.30.1.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -3812,7 +3812,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `local`</t>
+          <t>Verifying `20.30.1.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -3829,7 +3829,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `local`</t>
+          <t>Verifying `1.0.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -3846,7 +3846,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `local`</t>
+          <t>Verifying `1.0.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -3863,7 +3863,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `local`</t>
+          <t>Verifying `1.1.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -3880,7 +3880,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `local`</t>
+          <t>Verifying `1.1.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -3897,7 +3897,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `local`</t>
+          <t>Verifying `2.0.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -3914,7 +3914,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `local`</t>
+          <t>Verifying `2.0.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -3931,7 +3931,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `local`</t>
+          <t>Verifying `2.1.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -3948,7 +3948,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `local`</t>
+          <t>Verifying `2.1.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -3965,7 +3965,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `local`</t>
+          <t>Verifying `3.0.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -3982,7 +3982,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `local`</t>
+          <t>Verifying `3.0.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -3999,7 +3999,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `local`</t>
+          <t>Verifying `3.1.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -4016,7 +4016,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `root`</t>
+          <t>Verifying `3.1.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -4033,7 +4033,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `root`</t>
+          <t>Verifying `3.2.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -4050,7 +4050,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `root`</t>
+          <t>Verifying `3.2.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -4067,7 +4067,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `root`</t>
+          <t>Verifying `10.20.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -4084,7 +4084,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `root`</t>
+          <t>Verifying `10.20.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -4101,7 +4101,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `root`</t>
+          <t>Verifying `10.20.1.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `root`</t>
+          <t>Verifying `10.20.1.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `root`</t>
+          <t>Verifying `20.30.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -4152,7 +4152,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `root`</t>
+          <t>Verifying `20.30.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -4169,7 +4169,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `root`</t>
+          <t>Verifying `20.30.1.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -4186,7 +4186,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `root`</t>
+          <t>Verifying `20.30.1.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -4203,7 +4203,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `root`</t>
+          <t>Verifying `1.0.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -4220,7 +4220,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `root`</t>
+          <t>Verifying `1.0.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -4237,7 +4237,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `root`</t>
+          <t>Verifying `1.1.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -4254,7 +4254,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `root`</t>
+          <t>Verifying `1.1.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -4271,7 +4271,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `root`</t>
+          <t>Verifying `2.0.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -4288,7 +4288,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `root`</t>
+          <t>Verifying `2.0.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -4305,7 +4305,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `root`</t>
+          <t>Verifying `2.1.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -4322,7 +4322,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `root`</t>
+          <t>Verifying `2.1.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -4339,7 +4339,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `root`</t>
+          <t>Verifying `3.0.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -4356,7 +4356,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `root`</t>
+          <t>Verifying `3.0.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -4373,7 +4373,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `root`</t>
+          <t>Verifying `3.1.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -4390,7 +4390,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `net`</t>
+          <t>Verifying `3.1.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -4407,7 +4407,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `net`</t>
+          <t>Verifying `3.2.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -4424,7 +4424,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `net`</t>
+          <t>Verifying `3.2.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -4441,7 +4441,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `net`</t>
+          <t>Verifying `10.20.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -4458,7 +4458,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `net`</t>
+          <t>Verifying `10.20.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -4475,7 +4475,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `net`</t>
+          <t>Verifying `10.20.1.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -4492,7 +4492,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `net`</t>
+          <t>Verifying `10.20.1.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -4509,7 +4509,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `net`</t>
+          <t>Verifying `20.30.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -4526,7 +4526,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `net`</t>
+          <t>Verifying `20.30.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -4543,7 +4543,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `net`</t>
+          <t>Verifying `20.30.1.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -4560,7 +4560,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `net`</t>
+          <t>Verifying `20.30.1.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -4577,7 +4577,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `net`</t>
+          <t>Verifying `1.0.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -4594,7 +4594,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `net`</t>
+          <t>Verifying `1.0.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -4611,7 +4611,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `net`</t>
+          <t>Verifying `1.1.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -4628,7 +4628,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `net`</t>
+          <t>Verifying `1.1.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -4645,7 +4645,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `net`</t>
+          <t>Verifying `2.0.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -4662,7 +4662,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `net`</t>
+          <t>Verifying `2.0.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -4679,7 +4679,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `net`</t>
+          <t>Verifying `2.1.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -4696,7 +4696,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `net`</t>
+          <t>Verifying `2.1.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -4713,7 +4713,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `net`</t>
+          <t>Verifying `3.0.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -4730,7 +4730,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `net`</t>
+          <t>Verifying `3.0.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `net`</t>
+          <t>Verifying `3.1.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -4764,7 +4764,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `pc`</t>
+          <t>Verifying `3.1.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -4781,7 +4781,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `pc`</t>
+          <t>Verifying `3.2.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -4798,7 +4798,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `pc`</t>
+          <t>Verifying `3.2.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -4815,7 +4815,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `pc`</t>
+          <t>Verifying `10.20.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -4832,7 +4832,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `pc`</t>
+          <t>Verifying `10.20.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -4849,7 +4849,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `pc`</t>
+          <t>Verifying `10.20.1.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -4866,7 +4866,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `pc`</t>
+          <t>Verifying `10.20.1.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -4883,7 +4883,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `pc`</t>
+          <t>Verifying `20.30.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -4900,7 +4900,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `pc`</t>
+          <t>Verifying `20.30.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -4917,7 +4917,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `pc`</t>
+          <t>Verifying `20.30.1.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -4934,7 +4934,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `pc`</t>
+          <t>Verifying `20.30.1.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -4951,7 +4951,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `pc`</t>
+          <t>Verifying `1.0.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -4968,7 +4968,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `pc`</t>
+          <t>Verifying `1.0.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -4985,7 +4985,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `pc`</t>
+          <t>Verifying `1.1.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -5002,7 +5002,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `pc`</t>
+          <t>Verifying `1.1.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `pc`</t>
+          <t>Verifying `2.0.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -5036,7 +5036,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `pc`</t>
+          <t>Verifying `2.0.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -5053,7 +5053,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `pc`</t>
+          <t>Verifying `2.1.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -5070,7 +5070,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `pc`</t>
+          <t>Verifying `2.1.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -5087,7 +5087,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `pc`</t>
+          <t>Verifying `3.0.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -5104,7 +5104,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `pc`</t>
+          <t>Verifying `3.0.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -5121,7 +5121,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `pc`</t>
+          <t>Verifying `3.1.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -5138,7 +5138,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Checking that bgpd is running on device `as1r1`</t>
+          <t>Verifying `3.1.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -5155,7 +5155,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Checking that ripd is running on device `as1r1`</t>
+          <t>Verifying `3.2.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -5172,7 +5172,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Checking that bgpd is running on device `as1r2`</t>
+          <t>Verifying `3.2.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -5189,7 +5189,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Checking that ripd is running on device `as1r2`</t>
+          <t>Verifying `10.20.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -5206,7 +5206,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Checking that bgpd is running on device `as2r1`</t>
+          <t>Verifying `10.20.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -5223,7 +5223,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Checking that ripd is running on device `as2r1`</t>
+          <t>Verifying `10.20.1.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -5240,7 +5240,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Checking that bgpd is running on device `as2r2`</t>
+          <t>Verifying `10.20.1.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -5257,7 +5257,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Checking that ripd is running on device `as2r2`</t>
+          <t>Verifying `20.30.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -5274,7 +5274,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Checking that bgpd is running on device `as3r1`</t>
+          <t>Verifying `20.30.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -5291,7 +5291,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Checking that ripd is running on device `as3r1`</t>
+          <t>Verifying `20.30.1.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -5308,7 +5308,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Checking that bgpd is running on device `as3r2`</t>
+          <t>Verifying `20.30.1.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -5325,7 +5325,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Checking that ripd is running on device `as3r2`</t>
+          <t>Checking that bgpd is running on device `as1r1`</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -5342,7 +5342,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Checking that named is running on device `local`</t>
+          <t>Checking that ripd is running on device `as1r1`</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -5359,7 +5359,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `local`</t>
+          <t>Checking that bgpd is running on device `as1r2`</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -5376,7 +5376,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Checking that named is running on device `net`</t>
+          <t>Checking that ripd is running on device `as1r2`</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -5393,7 +5393,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `net`</t>
+          <t>Checking that bgpd is running on device `as2r1`</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -5410,7 +5410,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Checking that named is running on device `root`</t>
+          <t>Checking that ripd is running on device `as2r1`</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -5427,7 +5427,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `root`</t>
+          <t>Checking that bgpd is running on device `as2r2`</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -5444,7 +5444,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `pc`</t>
+          <t>Checking that ripd is running on device `as2r2`</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -5461,7 +5461,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>as1r1 has bgp peer 1.0.0.2</t>
+          <t>Checking that bgpd is running on device `as3r1`</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -5478,7 +5478,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>as1r1 has bgp peer 10.20.0.2</t>
+          <t>Checking that ripd is running on device `as3r1`</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -5495,7 +5495,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>as1r2 has bgp peer 1.0.0.1</t>
+          <t>Checking that bgpd is running on device `as3r2`</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -5512,7 +5512,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>as1r2 has bgp peer 10.20.1.2</t>
+          <t>Checking that ripd is running on device `as3r2`</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -5529,7 +5529,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>as2r1 has bgp peer 2.0.0.2</t>
+          <t>Checking that named is running on device `local`</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -5546,7 +5546,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>as2r1 has bgp peer 10.20.0.1</t>
+          <t>Checking that watchfrr is not running on device `local`</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -5563,7 +5563,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>as2r1 has bgp peer 20.30.0.2</t>
+          <t>Checking that named is running on device `net`</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -5580,7 +5580,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>as2r2 has bgp peer 2.0.0.1</t>
+          <t>Checking that watchfrr is not running on device `net`</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -5597,7 +5597,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>as2r2 has bgp peer 10.20.1.1</t>
+          <t>Checking that named is running on device `root`</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -5614,24 +5614,24 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>as2r2 has bgp peer 20.30.1.2</t>
+          <t>Checking that watchfrr is not running on device `root`</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>The peering between as2r2 and 20.30.1.2 is not up.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>as3r1 has bgp peer 3.0.0.2</t>
+          <t>Checking that watchfrr is not running on device `pc`</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -5648,7 +5648,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>as3r1 has bgp peer 20.30.0.1</t>
+          <t>as1r1 has bgp neighbor 1.0.0.2 AS1</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
@@ -5658,14 +5658,14 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as1r1 has neighbor 1.0.0.2 with ASN: 1</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>as3r2 has bgp peer 3.0.0.1</t>
+          <t>as1r1 has bgp neighbor 1.0.0.2 AS1 established</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -5682,24 +5682,24 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>as3r2 has bgp peer 20.30.1.1</t>
+          <t>as1r1 has bgp neighbor 10.20.0.2 AS2</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>The session is configured but is in the Active state</t>
+          <t>as1r1 has neighbor 10.20.0.2 with ASN: 2</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>Check bgpd network (1.0.0.0/8) for as1r1</t>
+          <t>as1r1 has bgp neighbor 10.20.0.2 AS2 established</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -5716,7 +5716,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Check bgpd network (1.0.0.0/8) for as1r2</t>
+          <t>as1r2 has bgp neighbor 1.0.0.1 AS1</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -5726,14 +5726,14 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as1r2 has neighbor 1.0.0.1 with ASN: 1</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Check bgpd network (2.0.0.0/8) for as2r1</t>
+          <t>as1r2 has bgp neighbor 1.0.0.1 AS1 established</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Check bgpd network (2.0.0.0/8) for as2r2</t>
+          <t>as1r2 has bgp neighbor 10.20.1.2 AS2</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -5760,14 +5760,14 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as1r2 has neighbor 10.20.1.2 with ASN: 2</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Check bgpd network (3.0.0.0/8) for as3r1</t>
+          <t>as1r2 has bgp neighbor 10.20.1.2 AS2 established</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -5784,7 +5784,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Check bgpd network (3.0.0.0/8) for as3r2</t>
+          <t>as2r1 has bgp neighbor 2.0.0.2 AS2</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -5794,14 +5794,14 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as2r1 has neighbor 2.0.0.2 with ASN: 2</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Checking that connected routes are not redistributed to bgpd on device `as1r1`</t>
+          <t>as2r1 has bgp neighbor 2.0.0.2 AS2 established</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -5818,7 +5818,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Checking that connected routes are not redistributed to bgpd on device `as1r2`</t>
+          <t>as2r1 has bgp neighbor 10.20.0.1 AS1</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -5828,14 +5828,14 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as2r1 has neighbor 10.20.0.1 with ASN: 1</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Checking that connected routes are not redistributed to bgpd on device `as2r1`</t>
+          <t>as2r1 has bgp neighbor 10.20.0.1 AS1 established</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -5852,7 +5852,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Checking that connected routes are not redistributed to bgpd on device `as2r2`</t>
+          <t>as2r1 has bgp neighbor 20.30.0.2 AS3</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -5862,14 +5862,14 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as2r1 has neighbor 20.30.0.2 with ASN: 3</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Checking that connected routes are not redistributed to bgpd on device `as3r1`</t>
+          <t>as2r1 has bgp neighbor 20.30.0.2 AS3 established</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -5886,7 +5886,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Checking that connected routes are not redistributed to bgpd on device `as3r2`</t>
+          <t>as2r2 has bgp neighbor 2.0.0.1 AS2</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -5896,14 +5896,14 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as2r2 has neighbor 2.0.0.1 with ASN: 2</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Checking that connected routes are redistributed to ripd on device `as1r1`</t>
+          <t>as2r2 has bgp neighbor 2.0.0.1 AS2 established</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -5920,7 +5920,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Checking that bgp routes are redistributed to ripd on device `as1r1`</t>
+          <t>as2r2 has bgp neighbor 10.20.1.1 AS1</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -5930,14 +5930,14 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as2r2 has neighbor 10.20.1.1 with ASN: 1</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Checking that connected routes are redistributed to ripd on device `as1r2`</t>
+          <t>as2r2 has bgp neighbor 10.20.1.1 AS1 established</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -5954,24 +5954,24 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>Checking that bgp routes are redistributed to ripd on device `as1r2`</t>
+          <t>Checking as2r2 BGP neighbors</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>The peering between as2r2 and 20.30.1.2 is not configured.</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Checking that connected routes are redistributed to ripd on device `as2r1`</t>
+          <t>as3r1 has bgp neighbor 3.0.0.2 AS3</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -5981,14 +5981,14 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as3r1 has neighbor 3.0.0.2 with ASN: 3</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>Checking that bgp routes are redistributed to ripd on device `as2r1`</t>
+          <t>as3r1 has bgp neighbor 3.0.0.2 AS3 established</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -6005,7 +6005,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>Checking that connected routes are redistributed to ripd on device `as2r2`</t>
+          <t>as3r1 has bgp neighbor 20.30.0.1 AS2</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -6015,14 +6015,14 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as3r1 has neighbor 20.30.0.1 with ASN: 2</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>Checking that bgp routes are redistributed to ripd on device `as2r2`</t>
+          <t>as3r1 has bgp neighbor 20.30.0.1 AS2 established</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -6039,7 +6039,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>Checking that connected routes are redistributed to ripd on device `as3r1`</t>
+          <t>as3r2 has bgp neighbor 3.0.0.1 AS3</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -6049,14 +6049,14 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as3r2 has neighbor 3.0.0.1 with ASN: 3</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Checking that bgp routes are redistributed to ripd on device `as3r1`</t>
+          <t>as3r2 has bgp neighbor 3.0.0.1 AS3 established</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -6073,7 +6073,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>Checking that connected routes are redistributed to ripd on device `as3r2`</t>
+          <t>as3r2 has bgp neighbor 20.30.1.1 AS2</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -6083,184 +6083,184 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>as3r2 has neighbor 20.30.1.1 with ASN: 2</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>Checking that bgp routes are redistributed to ripd on device `as3r2`</t>
+          <t>as3r2 has bgp neighbor 20.30.1.1 AS2</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>The session is configured but is in the Active state</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>Checking the routing table of as1r1</t>
+          <t>Check bgpd network (1.0.0.0/8) for as1r1</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>The routing table of as1r1 have the wrong number of routes: 6, expected: 8</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Checking the routing table of as1r2</t>
+          <t>Check bgpd network (1.0.0.0/8) for as1r2</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>The routing table of as1r2 have the wrong number of routes: 5, expected: 8</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Checking the routing table of as2r1</t>
+          <t>Check bgpd network (2.0.0.0/8) for as2r1</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>The routing table of as2r1 have the wrong number of routes: 5, expected: 8</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Checking the routing table of as2r2</t>
+          <t>Check bgpd network (2.0.0.0/8) for as2r2</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>The routing table of as2r2 have the wrong number of routes: 4, expected: 8</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Checking the routing table of as3r1</t>
+          <t>Check bgpd network (3.0.0.0/8) for as3r1</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>The routing table of as3r1 have the wrong number of routes: 7, expected: 9</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Checking the routing table of root</t>
+          <t>Check bgpd network (3.0.0.0/8) for as3r2</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>The routing table of root have the wrong number of routes: 1, expected: 2</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Checking the routing table of net</t>
+          <t>Checking that connected routes are not redistributed to bgpd on device `as1r1`</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>The routing table of net have the wrong number of routes: 1, expected: 2</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Checking the routing table of pc</t>
+          <t>Checking that connected routes are not redistributed to bgpd on device `as1r2`</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>The routing table of pc have the wrong number of routes: 1, expected: 2</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Checking the routing table of local</t>
+          <t>Checking that connected routes are not redistributed to bgpd on device `as2r1`</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>The routing table of local have the wrong number of routes: 1, expected: 2</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that connected routes are not redistributed to bgpd on device `as2r2`</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -6277,7 +6277,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that connected routes are not redistributed to bgpd on device `as3r1`</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -6294,7 +6294,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that connected routes are not redistributed to bgpd on device `as3r2`</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -6311,7 +6311,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
+          <t>Checking that connected routes are redistributed to ripd on device `as1r1`</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -6328,117 +6328,831 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
+          <t>Checking that bgp routes are redistributed to ripd on device `as1r1`</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r1`</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
+          <t>Checking that connected routes are redistributed to ripd on device `as1r2`</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r2`</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
+          <t>Checking that bgp routes are redistributed to ripd on device `as1r2`</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as2r1`</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
+          <t>Checking that connected routes are redistributed to ripd on device `as2r1`</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as2r2`</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
+          <t>Checking that bgp routes are redistributed to ripd on device `as2r1`</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as3r1`</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
+          <t>Checking that connected routes are redistributed to ripd on device `as2r2`</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as3r2`</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
+          <t>Checking that bgp routes are redistributed to ripd on device `as2r2`</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>Checking that connected routes are redistributed to ripd on device `as3r1`</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>Checking that bgp routes are redistributed to ripd on device `as3r1`</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>Checking that connected routes are redistributed to ripd on device `as3r2`</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>Checking that bgp routes are redistributed to ripd on device `as3r2`</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as1r1</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>The routing table of as1r1 have the wrong number of routes: 6, expected: 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as1r1</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>The routing table of as1r1 is missing route 1.0.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as1r1</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>The routing table of as1r1 is missing route 10.20.0.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as1r2</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>The routing table of as1r2 have the wrong number of routes: 5, expected: 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as1r2</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>The routing table of as1r2 is missing route 1.0.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as1r2</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>The routing table of as1r2 is missing route 1.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as1r2</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>The routing table of as1r2 is missing route 10.20.1.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r1</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>The routing table of as2r1 have the wrong number of routes: 5, expected: 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r1</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>The routing table of as2r1 is missing route 2.0.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r1</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>The routing table of as2r1 is missing route 10.20.0.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r1</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>The routing table of as2r1 is missing route 20.30.0.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r2</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>The routing table of as2r2 have the wrong number of routes: 4, expected: 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r2</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>The routing table of as2r2 is missing route 2.0.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r2</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>The routing table of as2r2 is missing route 2.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r2</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>The routing table of as2r2 is missing route 10.20.1.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r2</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>The routing table of as2r2 is missing route 20.30.1.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as3r1</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>The routing table of as3r1 have the wrong number of routes: 7, expected: 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as3r1</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>The routing table of as3r1 is missing route 3.0.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as3r1</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>The routing table of as3r1 is missing route 20.30.0.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>Checking the routing table of root</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>The routing table of root have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>Checking the routing table of root</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>The routing table of root is missing route 1.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>Checking the routing table of net</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>The routing table of net have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>Checking the routing table of net</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>The routing table of net is missing route 2.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Checking the routing table of pc</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>The routing table of pc have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Checking the routing table of pc</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>The routing table of pc is missing route 3.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Checking the routing table of local</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>The routing table of local have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>Checking the routing table of local</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>The routing table of local is missing route 3.2.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as1r1`</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as1r2`</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as2r1`</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as2r2`</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as3r1`</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as3r2`</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
           <t>Checking that `3.2.0.2` is the local name server for device `pc`</t>
         </is>
       </c>
-      <c r="B351" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="C351" t="inlineStr">
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -6455,7 +7169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6483,7 +7197,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>as2r2 has bgp peer 20.30.1.2</t>
+          <t>Checking as2r2 BGP neighbors</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6493,14 +7207,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The peering between as2r2 and 20.30.1.2 is not up.</t>
+          <t>The peering between as2r2 and 20.30.1.2 is not configured.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>as3r2 has bgp peer 20.30.1.1</t>
+          <t>as3r2 has bgp neighbor 20.30.1.1 AS2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -6534,7 +7248,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Checking the routing table of as1r2</t>
+          <t>Checking the routing table of as1r1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -6544,14 +7258,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>The routing table of as1r2 have the wrong number of routes: 5, expected: 8</t>
+          <t>The routing table of as1r1 is missing route 1.0.0.0/24</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Checking the routing table of as2r1</t>
+          <t>Checking the routing table of as1r1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -6561,14 +7275,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>The routing table of as2r1 have the wrong number of routes: 5, expected: 8</t>
+          <t>The routing table of as1r1 is missing route 10.20.0.0/30</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Checking the routing table of as2r2</t>
+          <t>Checking the routing table of as1r2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -6578,14 +7292,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>The routing table of as2r2 have the wrong number of routes: 4, expected: 8</t>
+          <t>The routing table of as1r2 have the wrong number of routes: 5, expected: 8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Checking the routing table of as3r1</t>
+          <t>Checking the routing table of as1r2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -6595,14 +7309,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The routing table of as3r1 have the wrong number of routes: 7, expected: 9</t>
+          <t>The routing table of as1r2 is missing route 1.0.0.0/24</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Checking the routing table of root</t>
+          <t>Checking the routing table of as1r2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -6612,14 +7326,14 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>The routing table of root have the wrong number of routes: 1, expected: 2</t>
+          <t>The routing table of as1r2 is missing route 1.1.0.0/24</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Checking the routing table of net</t>
+          <t>Checking the routing table of as1r2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -6629,14 +7343,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>The routing table of net have the wrong number of routes: 1, expected: 2</t>
+          <t>The routing table of as1r2 is missing route 10.20.1.0/30</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Checking the routing table of pc</t>
+          <t>Checking the routing table of as2r1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -6646,14 +7360,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>The routing table of pc have the wrong number of routes: 1, expected: 2</t>
+          <t>The routing table of as2r1 have the wrong number of routes: 5, expected: 8</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Checking the routing table of local</t>
+          <t>Checking the routing table of as2r1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -6663,14 +7377,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>The routing table of local have the wrong number of routes: 1, expected: 2</t>
+          <t>The routing table of as2r1 is missing route 2.0.0.0/24</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
+          <t>Checking the routing table of as2r1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -6680,14 +7394,14 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r1`</t>
+          <t>The routing table of as2r1 is missing route 10.20.0.0/30</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
+          <t>Checking the routing table of as2r1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -6697,14 +7411,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r2`</t>
+          <t>The routing table of as2r1 is missing route 20.30.0.0/30</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
+          <t>Checking the routing table of as2r2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -6714,14 +7428,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as2r1`</t>
+          <t>The routing table of as2r2 have the wrong number of routes: 4, expected: 8</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
+          <t>Checking the routing table of as2r2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -6731,14 +7445,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as2r2`</t>
+          <t>The routing table of as2r2 is missing route 2.0.0.0/24</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
+          <t>Checking the routing table of as2r2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -6748,22 +7462,328 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as3r1`</t>
+          <t>The routing table of as2r2 is missing route 2.1.0.0/24</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Checking the routing table of as2r2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>The routing table of as2r2 is missing route 10.20.1.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as2r2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>The routing table of as2r2 is missing route 20.30.1.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as3r1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>The routing table of as3r1 have the wrong number of routes: 7, expected: 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as3r1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>The routing table of as3r1 is missing route 3.0.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Checking the routing table of as3r1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>The routing table of as3r1 is missing route 20.30.0.0/30</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Checking the routing table of root</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>The routing table of root have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Checking the routing table of root</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>The routing table of root is missing route 1.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Checking the routing table of net</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>The routing table of net have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Checking the routing table of net</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>The routing table of net is missing route 2.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Checking the routing table of pc</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>The routing table of pc have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Checking the routing table of pc</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>The routing table of pc is missing route 3.1.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Checking the routing table of local</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>The routing table of local have the wrong number of routes: 1, expected: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Checking the routing table of local</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>The routing table of local is missing route 3.2.0.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as1r1`</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as1r2`</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as2r1`</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as2r2`</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>`resolv.conf` file not found for device `as3r1`</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B36" t="inlineStr">
         <is>
           <t>False</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>`resolv.conf` file not found for device `as3r2`</t>
         </is>

</xml_diff>